<commit_message>
Rescoring of the Van Delden Protocol
Scores updated in TIDIER Van Delden paper based on the published
protocol. All analyses and figures re-run.
</commit_message>
<xml_diff>
--- a/group_desc/data_GROUPS_protocols_added.xlsx
+++ b/group_desc/data_GROUPS_protocols_added.xlsx
@@ -3688,7 +3688,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AD1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A391" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AS407" sqref="AS407"/>
+      <selection pane="bottomLeft" activeCell="AL405" sqref="AL405"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -57765,10 +57765,10 @@
         <v>1</v>
       </c>
       <c r="AM405" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN405" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO405" s="27">
         <v>1</v>
@@ -57787,7 +57787,7 @@
       </c>
       <c r="AT405" s="71">
         <f t="shared" si="61"/>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="406" spans="1:46" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -57904,10 +57904,10 @@
         <v>1</v>
       </c>
       <c r="AM406" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN406" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO406" s="27">
         <v>1</v>
@@ -57926,7 +57926,7 @@
       </c>
       <c r="AT406" s="71">
         <f t="shared" si="61"/>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="407" spans="1:46" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -58046,7 +58046,7 @@
         <v>1</v>
       </c>
       <c r="AN407" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO407" s="27">
         <v>1</v>
@@ -58065,7 +58065,7 @@
       </c>
       <c r="AT407" s="71">
         <f t="shared" si="61"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="408" spans="1:46" s="95" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>